<commit_message>
Leaderboard xlsx file updated
</commit_message>
<xml_diff>
--- a/src/leaderboard.xlsx
+++ b/src/leaderboard.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\HP\Works\robomania\Leaderboard\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmtir\Desktop\leaderboard\Leaderboard\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD1C162-6B36-4C25-A91C-8CD55C47816D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8FB2C0-959D-4057-A368-B1A65226BB5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8B23C945-1180-4F52-B938-814F22B23B0E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{8B23C945-1180-4F52-B938-814F22B23B0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,27 +34,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>teamName</t>
   </si>
   <si>
-    <t>points</t>
-  </si>
-  <si>
     <t>round 1</t>
   </si>
   <si>
     <t>round 2</t>
   </si>
   <si>
-    <t>Polymath</t>
-  </si>
-  <si>
-    <t>xyz</t>
-  </si>
-  <si>
-    <t>tirmanwar</t>
+    <t>RCB</t>
+  </si>
+  <si>
+    <t>Santoor Dads</t>
+  </si>
+  <si>
+    <t>DD</t>
+  </si>
+  <si>
+    <t>Rewind</t>
+  </si>
+  <si>
+    <t>Lakshya</t>
+  </si>
+  <si>
+    <t>Dynamic Duo</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>A square</t>
+  </si>
+  <si>
+    <t>Immortal</t>
+  </si>
+  <si>
+    <t>Dwe Pra</t>
+  </si>
+  <si>
+    <t>Team Unity</t>
+  </si>
+  <si>
+    <t>DeO Data Science</t>
+  </si>
+  <si>
+    <t>SB K2D</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Parle-G</t>
+  </si>
+  <si>
+    <t>NAN</t>
   </si>
 </sst>
 </file>
@@ -98,10 +134,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -120,9 +156,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -160,7 +196,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -266,7 +302,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -408,7 +444,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -416,125 +452,321 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A04473FF-BE4A-48AC-986B-6EC2C1DF0E4F}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.88671875" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.88671875" customWidth="1"/>
     <col min="4" max="4" width="21.5546875" customWidth="1"/>
     <col min="5" max="5" width="22.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="B2">
+        <v>822</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>35</v>
+      </c>
+      <c r="F2">
+        <v>822</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.5708333333333333</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>680</v>
+      </c>
+      <c r="E3">
+        <v>50</v>
+      </c>
+      <c r="F3">
+        <v>680</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.47222222222222227</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>670</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>670</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.46527777777777773</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>565</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>565</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.3923611111111111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>640</v>
+      </c>
+      <c r="E6">
+        <v>80</v>
+      </c>
+      <c r="F6">
+        <v>640</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.44444444444444442</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>400</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>400</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.27777777777777779</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>700</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>700</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.4861111111111111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
-        <v>4.3</v>
-      </c>
-      <c r="E2">
+      <c r="B9">
+        <v>667</v>
+      </c>
+      <c r="E9">
+        <v>60</v>
+      </c>
+      <c r="F9">
+        <v>667</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.46319444444444446</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>580</v>
+      </c>
+      <c r="E10">
+        <v>20</v>
+      </c>
+      <c r="F10">
+        <v>580</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.40277777777777773</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>885</v>
+      </c>
+      <c r="E11">
+        <v>30</v>
+      </c>
+      <c r="F11">
+        <v>885</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.61458333333333337</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>96</v>
+      </c>
+      <c r="B13">
+        <v>900</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13">
+        <v>900</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>69</v>
+      </c>
+      <c r="B14">
+        <v>880</v>
+      </c>
+      <c r="E14">
+        <v>35</v>
+      </c>
+      <c r="F14">
+        <v>880</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.61111111111111105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
+      <c r="B15">
+        <v>890</v>
+      </c>
+      <c r="E15">
+        <v>65</v>
+      </c>
+      <c r="F15">
+        <v>890</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.61805555555555558</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
+      <c r="A17" s="1"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
+      <c r="A18" s="1"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
+      <c r="A19" s="1"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
+      <c r="A20" s="1"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
+      <c r="A21" s="1"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
+      <c r="A22" s="1"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
+      <c r="A24" s="1"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
+      <c r="A25" s="1"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B23">
+    <sortCondition descending="1" ref="B2:B23"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>